<commit_message>
#3 When the 'bondsnummer' field is empty skip the record and continue
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/data.xlsx
+++ b/src/test/resources/testdata/data.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Export_Tennisvereniging_Tegenbo!$A$1:$AA$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Export_Tennisvereniging_Tegenbo!$A$1:$AA$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Export_Tennisvereniging_Tegenbo!$A$1:$AA$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Export_Tennisvereniging_Tegenbo!$A$1:$AA$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -210,7 +211,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -241,12 +242,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -307,7 +302,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -334,28 +329,28 @@
   </sheetPr>
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.0364372469636"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6842105263158"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.0566801619433"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.0728744939271"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1619433198381"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.20647773279352"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.7327935222672"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.6234817813765"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="31.3441295546559"/>
-    <col collapsed="false" hidden="false" max="21" min="17" style="0" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="26.8097165991903"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6518218623482"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.5425101214575"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.663967611336"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.3684210526316"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.9271255060729"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.5263157894737"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.44939271255061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9757085020243"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="32.0728744939271"/>
+    <col collapsed="false" hidden="false" max="21" min="17" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,9 +602,6 @@
       </c>
       <c r="R4" s="0" t="n">
         <v>10603</v>
-      </c>
-      <c r="S4" s="0" t="n">
-        <v>11224455</v>
       </c>
       <c r="T4" s="0" t="s">
         <v>35</v>

</xml_diff>